<commit_message>
dicionario de dados atualizado
</commit_message>
<xml_diff>
--- a/Documentos/xml's/dicionario-de-dados.xlsx
+++ b/Documentos/xml's/dicionario-de-dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\docs-faculdade\xml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\20201-3adsa-grupo1\Documentos\xml's\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>Nome do Atributo</t>
   </si>
@@ -144,6 +144,54 @@
   </si>
   <si>
     <t>Chave estrangeira referente as paradas das viagens</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>idPost</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>likes</t>
+  </si>
+  <si>
+    <t>Viagem_idViagem</t>
+  </si>
+  <si>
+    <t>Id fornecido para identificação do post</t>
+  </si>
+  <si>
+    <t>Titulo do post postado pelo usuario</t>
+  </si>
+  <si>
+    <t>Descrição do post fornecida pelo usuario</t>
+  </si>
+  <si>
+    <t>Numero de likes que o post recebeu</t>
+  </si>
+  <si>
+    <t>Chave estrangeira referente aos Usuarios e seus post's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chave estrangeira referente aos Post de viagens </t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>Post_idPost</t>
+  </si>
+  <si>
+    <t>Chave estrangeira referente aos posts e seu identificador</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -788,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1031,6 +1079,130 @@
         <v>3</v>
       </c>
     </row>
+    <row r="26" spans="1:3" ht="21" thickBot="1">
+      <c r="A26" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A27" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75">
+      <c r="A28" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75">
+      <c r="A29" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75">
+      <c r="A30" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75">
+      <c r="A31" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75">
+      <c r="A32" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75">
+      <c r="A33" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="21" thickBot="1">
+      <c r="A35" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A36" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75">
+      <c r="A37" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75">
+      <c r="A38" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="45" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>